<commit_message>
Quitado harcodeos y arreglado secuencia Mover Excel
</commit_message>
<xml_diff>
--- a/Proyecto_Final_Performer/Data/Config.xlsx
+++ b/Proyecto_Final_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgnte\Documents\UiPath\workspace\Proyecto_Final_Dispatcher\Proyecto_Final_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A90E29-AAAB-4511-AF5F-EABAD6CFBFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B114D6B8-3CF5-44B5-ABC8-75EDD7EE57CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4224" yWindow="1944" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5268" yWindow="2436" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -185,10 +185,10 @@
     <t>Output_Vendors</t>
   </si>
   <si>
-    <t>C:\Users\bgnte\Downloads\Vendor List.xlsx</t>
-  </si>
-  <si>
-    <t>Vendor_List</t>
+    <t>C:\Output_Vendors</t>
+  </si>
+  <si>
+    <t>output_Vendors_Path</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Añadido envío de correo
</commit_message>
<xml_diff>
--- a/Proyecto_Final_Performer/Data/Config.xlsx
+++ b/Proyecto_Final_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgnte\Documents\UiPath\workspace\Proyecto_Final_Dispatcher\Proyecto_Final_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BB3B82-D480-4ECA-85C2-CD1CB4A5762A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618DB504-CA6B-48BC-ADA6-894C952F2B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4224" yWindow="1944" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5484" yWindow="1140" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -192,6 +192,27 @@
   </si>
   <si>
     <t>in_Search_url</t>
+  </si>
+  <si>
+    <t>bgntejada@gmail.com</t>
+  </si>
+  <si>
+    <t>in_to_email</t>
+  </si>
+  <si>
+    <t>in_email_body</t>
+  </si>
+  <si>
+    <t>Adjunto el fichero con los resultados</t>
+  </si>
+  <si>
+    <t>in_email_subject</t>
+  </si>
+  <si>
+    <t>Dpto Contabilidad Facturas Cuentas</t>
+  </si>
+  <si>
+    <t>in_from_email</t>
   </si>
 </sst>
 </file>
@@ -579,7 +600,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -704,10 +725,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1694,9 +1743,11 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" xr:uid="{7E526D27-507D-48FB-8A02-22C87171E1B1}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{50392A95-EEFA-441F-9B94-CA1D9703E4E4}"/>
+    <hyperlink ref="B15" r:id="rId3" xr:uid="{2572081C-6038-4D86-B3E8-A20AF4D0F604}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2867,7 +2918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>